<commit_message>
completes the input framework for the last exercise
</commit_message>
<xml_diff>
--- a/ReFramework/UiDemo2/CalculateClientSecurityHash/Data/Config.xlsx
+++ b/ReFramework/UiDemo2/CalculateClientSecurityHash/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -36,7 +36,7 @@
     <t xml:space="preserve">System1URL</t>
   </si>
   <si>
-    <t xml:space="preserve">https://acme-test.uipath.com </t>
+    <t xml:space="preserve">“https://acme-test.uipath.com”</t>
   </si>
   <si>
     <t xml:space="preserve">Work website</t>
@@ -45,18 +45,12 @@
     <t xml:space="preserve">Sha1OnlineURL</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.sha1-online.com/</t>
+    <t xml:space="preserve">“http://www.sha1-online.com/”</t>
   </si>
   <si>
     <t xml:space="preserve">Sha1 generator</t>
   </si>
   <si>
-    <t xml:space="preserve">UiP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logF_BusinessProcessName</t>
-  </si>
-  <si>
     <t xml:space="preserve">MaxRetryNumber</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
   </si>
   <si>
     <t xml:space="preserve">Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“System1Credential”</t>
   </si>
   <si>
     <t xml:space="preserve">System1Credential</t>
@@ -193,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -220,12 +211,6 @@
       <b val="true"/>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -273,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -284,10 +269,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -313,8 +294,8 @@
   </sheetPr>
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -382,17 +363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1387,8 +1358,7 @@
     <row r="997" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://acme-test.uipath.com "/>
-    <hyperlink ref="B3" r:id="rId2" display="http://www.sha1-online.com/"/>
+    <hyperlink ref="B3" r:id="rId1" display="“http://www.sha1-online.com/”"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1456,178 +1426,178 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5000</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>30000</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>120000</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>15000</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>60000</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.6</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.8</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2625,8 +2595,8 @@
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2640,10 +2610,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2670,14 +2640,14 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>52</v>
+      <c r="A2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>